<commit_message>
Add improvements to project
</commit_message>
<xml_diff>
--- a/src/main/java/TestData/TestData.xlsx
+++ b/src/main/java/TestData/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\Epam\src\main\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB93D8F-CDB3-4A80-BC61-9AE6C39CCCF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707DEC1C-5282-4FDA-9271-3A263EADEDCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8640DDCA-E8BB-41F3-AE59-0D159B43E88A}"/>
   </bookViews>
@@ -39,10 +39,10 @@
     <t>george r. r. martin</t>
   </si>
   <si>
-    <t>Author FullName</t>
+    <t>Author Full Name</t>
   </si>
   <si>
-    <t>haruki murakami</t>
+    <t>theodore dreiser</t>
   </si>
 </sst>
 </file>
@@ -397,7 +397,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,5 +422,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>